<commit_message>
Dummy python working correctly.
</commit_message>
<xml_diff>
--- a/docs/output/OutputDataDefinition.xlsx
+++ b/docs/output/OutputDataDefinition.xlsx
@@ -1,54 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdpar\vs_code_repos\data-request-builder\docs\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D3B4BB4-15A1-4DF7-801C-2A533483679B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21525" windowHeight="11775" xr2:uid="{2DCE42E8-1CB8-4E01-9F5A-7226D1BF3895}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1560" yWindow="1560" windowWidth="21525" windowHeight="11775" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -67,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -381,13 +419,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81871C13-3D2E-4CA5-88E4-E344FB3EA8E2}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Will</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>cool</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Python now talks to JS.
</commit_message>
<xml_diff>
--- a/docs/output/OutputDataDefinition.xlsx
+++ b/docs/output/OutputDataDefinition.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1560" yWindow="1560" windowWidth="21525" windowHeight="11775" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -424,13 +424,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -450,6 +450,27 @@
       <c r="A3" t="inlineStr">
         <is>
           <t>cool</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>and</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>smart</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>and stuff</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Outputting table names to excel file.
</commit_message>
<xml_diff>
--- a/docs/output/OutputDataDefinition.xlsx
+++ b/docs/output/OutputDataDefinition.xlsx
@@ -1,33 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdpar\vs_code_repos\data-request-builder\docs\output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BAE101-A1D1-4780-BC5E-E75AA37F1610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Table_Names" sheetId="1" r:id="rId1"/>
+    <sheet name="Field_Names" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,80 +63,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -419,62 +377,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Will</t>
-        </is>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>cool</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>and</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>smart</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>and stuff</t>
-        </is>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fixes. Write to Excel using relative path
</commit_message>
<xml_diff>
--- a/docs/output/OutputDataDefinition.xlsx
+++ b/docs/output/OutputDataDefinition.xlsx
@@ -1,50 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdpar\vs_code_repos\data-request-builder\docs\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BAE101-A1D1-4780-BC5E-E75AA37F1610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Table_Names" sheetId="1" r:id="rId1"/>
-    <sheet name="Field_Names" sheetId="2" r:id="rId2"/>
+    <sheet name="Table_Names" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Field_Names" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -63,21 +47,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -377,38 +420,275 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
       </c>
     </row>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>T1F1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>T1F2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>T2F1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>T2F2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Groundwork for Python checkbox logic
</commit_message>
<xml_diff>
--- a/docs/output/OutputDataDefinition.xlsx
+++ b/docs/output/OutputDataDefinition.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A100"/>
+  <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
@@ -545,6 +545,906 @@
     <row r="98"/>
     <row r="99"/>
     <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
+    <row r="170"/>
+    <row r="171"/>
+    <row r="172"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189"/>
+    <row r="190"/>
+    <row r="191"/>
+    <row r="192"/>
+    <row r="193"/>
+    <row r="194"/>
+    <row r="195"/>
+    <row r="196"/>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200"/>
+    <row r="201"/>
+    <row r="202"/>
+    <row r="203"/>
+    <row r="204"/>
+    <row r="205"/>
+    <row r="206"/>
+    <row r="207"/>
+    <row r="208"/>
+    <row r="209"/>
+    <row r="210"/>
+    <row r="211"/>
+    <row r="212"/>
+    <row r="213"/>
+    <row r="214"/>
+    <row r="215"/>
+    <row r="216"/>
+    <row r="217"/>
+    <row r="218"/>
+    <row r="219"/>
+    <row r="220"/>
+    <row r="221"/>
+    <row r="222"/>
+    <row r="223"/>
+    <row r="224"/>
+    <row r="225"/>
+    <row r="226"/>
+    <row r="227"/>
+    <row r="228"/>
+    <row r="229"/>
+    <row r="230"/>
+    <row r="231"/>
+    <row r="232"/>
+    <row r="233"/>
+    <row r="234"/>
+    <row r="235"/>
+    <row r="236"/>
+    <row r="237"/>
+    <row r="238"/>
+    <row r="239"/>
+    <row r="240"/>
+    <row r="241"/>
+    <row r="242"/>
+    <row r="243"/>
+    <row r="244"/>
+    <row r="245"/>
+    <row r="246"/>
+    <row r="247"/>
+    <row r="248"/>
+    <row r="249"/>
+    <row r="250"/>
+    <row r="251"/>
+    <row r="252"/>
+    <row r="253"/>
+    <row r="254"/>
+    <row r="255"/>
+    <row r="256"/>
+    <row r="257"/>
+    <row r="258"/>
+    <row r="259"/>
+    <row r="260"/>
+    <row r="261"/>
+    <row r="262"/>
+    <row r="263"/>
+    <row r="264"/>
+    <row r="265"/>
+    <row r="266"/>
+    <row r="267"/>
+    <row r="268"/>
+    <row r="269"/>
+    <row r="270"/>
+    <row r="271"/>
+    <row r="272"/>
+    <row r="273"/>
+    <row r="274"/>
+    <row r="275"/>
+    <row r="276"/>
+    <row r="277"/>
+    <row r="278"/>
+    <row r="279"/>
+    <row r="280"/>
+    <row r="281"/>
+    <row r="282"/>
+    <row r="283"/>
+    <row r="284"/>
+    <row r="285"/>
+    <row r="286"/>
+    <row r="287"/>
+    <row r="288"/>
+    <row r="289"/>
+    <row r="290"/>
+    <row r="291"/>
+    <row r="292"/>
+    <row r="293"/>
+    <row r="294"/>
+    <row r="295"/>
+    <row r="296"/>
+    <row r="297"/>
+    <row r="298"/>
+    <row r="299"/>
+    <row r="300"/>
+    <row r="301"/>
+    <row r="302"/>
+    <row r="303"/>
+    <row r="304"/>
+    <row r="305"/>
+    <row r="306"/>
+    <row r="307"/>
+    <row r="308"/>
+    <row r="309"/>
+    <row r="310"/>
+    <row r="311"/>
+    <row r="312"/>
+    <row r="313"/>
+    <row r="314"/>
+    <row r="315"/>
+    <row r="316"/>
+    <row r="317"/>
+    <row r="318"/>
+    <row r="319"/>
+    <row r="320"/>
+    <row r="321"/>
+    <row r="322"/>
+    <row r="323"/>
+    <row r="324"/>
+    <row r="325"/>
+    <row r="326"/>
+    <row r="327"/>
+    <row r="328"/>
+    <row r="329"/>
+    <row r="330"/>
+    <row r="331"/>
+    <row r="332"/>
+    <row r="333"/>
+    <row r="334"/>
+    <row r="335"/>
+    <row r="336"/>
+    <row r="337"/>
+    <row r="338"/>
+    <row r="339"/>
+    <row r="340"/>
+    <row r="341"/>
+    <row r="342"/>
+    <row r="343"/>
+    <row r="344"/>
+    <row r="345"/>
+    <row r="346"/>
+    <row r="347"/>
+    <row r="348"/>
+    <row r="349"/>
+    <row r="350"/>
+    <row r="351"/>
+    <row r="352"/>
+    <row r="353"/>
+    <row r="354"/>
+    <row r="355"/>
+    <row r="356"/>
+    <row r="357"/>
+    <row r="358"/>
+    <row r="359"/>
+    <row r="360"/>
+    <row r="361"/>
+    <row r="362"/>
+    <row r="363"/>
+    <row r="364"/>
+    <row r="365"/>
+    <row r="366"/>
+    <row r="367"/>
+    <row r="368"/>
+    <row r="369"/>
+    <row r="370"/>
+    <row r="371"/>
+    <row r="372"/>
+    <row r="373"/>
+    <row r="374"/>
+    <row r="375"/>
+    <row r="376"/>
+    <row r="377"/>
+    <row r="378"/>
+    <row r="379"/>
+    <row r="380"/>
+    <row r="381"/>
+    <row r="382"/>
+    <row r="383"/>
+    <row r="384"/>
+    <row r="385"/>
+    <row r="386"/>
+    <row r="387"/>
+    <row r="388"/>
+    <row r="389"/>
+    <row r="390"/>
+    <row r="391"/>
+    <row r="392"/>
+    <row r="393"/>
+    <row r="394"/>
+    <row r="395"/>
+    <row r="396"/>
+    <row r="397"/>
+    <row r="398"/>
+    <row r="399"/>
+    <row r="400"/>
+    <row r="401"/>
+    <row r="402"/>
+    <row r="403"/>
+    <row r="404"/>
+    <row r="405"/>
+    <row r="406"/>
+    <row r="407"/>
+    <row r="408"/>
+    <row r="409"/>
+    <row r="410"/>
+    <row r="411"/>
+    <row r="412"/>
+    <row r="413"/>
+    <row r="414"/>
+    <row r="415"/>
+    <row r="416"/>
+    <row r="417"/>
+    <row r="418"/>
+    <row r="419"/>
+    <row r="420"/>
+    <row r="421"/>
+    <row r="422"/>
+    <row r="423"/>
+    <row r="424"/>
+    <row r="425"/>
+    <row r="426"/>
+    <row r="427"/>
+    <row r="428"/>
+    <row r="429"/>
+    <row r="430"/>
+    <row r="431"/>
+    <row r="432"/>
+    <row r="433"/>
+    <row r="434"/>
+    <row r="435"/>
+    <row r="436"/>
+    <row r="437"/>
+    <row r="438"/>
+    <row r="439"/>
+    <row r="440"/>
+    <row r="441"/>
+    <row r="442"/>
+    <row r="443"/>
+    <row r="444"/>
+    <row r="445"/>
+    <row r="446"/>
+    <row r="447"/>
+    <row r="448"/>
+    <row r="449"/>
+    <row r="450"/>
+    <row r="451"/>
+    <row r="452"/>
+    <row r="453"/>
+    <row r="454"/>
+    <row r="455"/>
+    <row r="456"/>
+    <row r="457"/>
+    <row r="458"/>
+    <row r="459"/>
+    <row r="460"/>
+    <row r="461"/>
+    <row r="462"/>
+    <row r="463"/>
+    <row r="464"/>
+    <row r="465"/>
+    <row r="466"/>
+    <row r="467"/>
+    <row r="468"/>
+    <row r="469"/>
+    <row r="470"/>
+    <row r="471"/>
+    <row r="472"/>
+    <row r="473"/>
+    <row r="474"/>
+    <row r="475"/>
+    <row r="476"/>
+    <row r="477"/>
+    <row r="478"/>
+    <row r="479"/>
+    <row r="480"/>
+    <row r="481"/>
+    <row r="482"/>
+    <row r="483"/>
+    <row r="484"/>
+    <row r="485"/>
+    <row r="486"/>
+    <row r="487"/>
+    <row r="488"/>
+    <row r="489"/>
+    <row r="490"/>
+    <row r="491"/>
+    <row r="492"/>
+    <row r="493"/>
+    <row r="494"/>
+    <row r="495"/>
+    <row r="496"/>
+    <row r="497"/>
+    <row r="498"/>
+    <row r="499"/>
+    <row r="500"/>
+    <row r="501"/>
+    <row r="502"/>
+    <row r="503"/>
+    <row r="504"/>
+    <row r="505"/>
+    <row r="506"/>
+    <row r="507"/>
+    <row r="508"/>
+    <row r="509"/>
+    <row r="510"/>
+    <row r="511"/>
+    <row r="512"/>
+    <row r="513"/>
+    <row r="514"/>
+    <row r="515"/>
+    <row r="516"/>
+    <row r="517"/>
+    <row r="518"/>
+    <row r="519"/>
+    <row r="520"/>
+    <row r="521"/>
+    <row r="522"/>
+    <row r="523"/>
+    <row r="524"/>
+    <row r="525"/>
+    <row r="526"/>
+    <row r="527"/>
+    <row r="528"/>
+    <row r="529"/>
+    <row r="530"/>
+    <row r="531"/>
+    <row r="532"/>
+    <row r="533"/>
+    <row r="534"/>
+    <row r="535"/>
+    <row r="536"/>
+    <row r="537"/>
+    <row r="538"/>
+    <row r="539"/>
+    <row r="540"/>
+    <row r="541"/>
+    <row r="542"/>
+    <row r="543"/>
+    <row r="544"/>
+    <row r="545"/>
+    <row r="546"/>
+    <row r="547"/>
+    <row r="548"/>
+    <row r="549"/>
+    <row r="550"/>
+    <row r="551"/>
+    <row r="552"/>
+    <row r="553"/>
+    <row r="554"/>
+    <row r="555"/>
+    <row r="556"/>
+    <row r="557"/>
+    <row r="558"/>
+    <row r="559"/>
+    <row r="560"/>
+    <row r="561"/>
+    <row r="562"/>
+    <row r="563"/>
+    <row r="564"/>
+    <row r="565"/>
+    <row r="566"/>
+    <row r="567"/>
+    <row r="568"/>
+    <row r="569"/>
+    <row r="570"/>
+    <row r="571"/>
+    <row r="572"/>
+    <row r="573"/>
+    <row r="574"/>
+    <row r="575"/>
+    <row r="576"/>
+    <row r="577"/>
+    <row r="578"/>
+    <row r="579"/>
+    <row r="580"/>
+    <row r="581"/>
+    <row r="582"/>
+    <row r="583"/>
+    <row r="584"/>
+    <row r="585"/>
+    <row r="586"/>
+    <row r="587"/>
+    <row r="588"/>
+    <row r="589"/>
+    <row r="590"/>
+    <row r="591"/>
+    <row r="592"/>
+    <row r="593"/>
+    <row r="594"/>
+    <row r="595"/>
+    <row r="596"/>
+    <row r="597"/>
+    <row r="598"/>
+    <row r="599"/>
+    <row r="600"/>
+    <row r="601"/>
+    <row r="602"/>
+    <row r="603"/>
+    <row r="604"/>
+    <row r="605"/>
+    <row r="606"/>
+    <row r="607"/>
+    <row r="608"/>
+    <row r="609"/>
+    <row r="610"/>
+    <row r="611"/>
+    <row r="612"/>
+    <row r="613"/>
+    <row r="614"/>
+    <row r="615"/>
+    <row r="616"/>
+    <row r="617"/>
+    <row r="618"/>
+    <row r="619"/>
+    <row r="620"/>
+    <row r="621"/>
+    <row r="622"/>
+    <row r="623"/>
+    <row r="624"/>
+    <row r="625"/>
+    <row r="626"/>
+    <row r="627"/>
+    <row r="628"/>
+    <row r="629"/>
+    <row r="630"/>
+    <row r="631"/>
+    <row r="632"/>
+    <row r="633"/>
+    <row r="634"/>
+    <row r="635"/>
+    <row r="636"/>
+    <row r="637"/>
+    <row r="638"/>
+    <row r="639"/>
+    <row r="640"/>
+    <row r="641"/>
+    <row r="642"/>
+    <row r="643"/>
+    <row r="644"/>
+    <row r="645"/>
+    <row r="646"/>
+    <row r="647"/>
+    <row r="648"/>
+    <row r="649"/>
+    <row r="650"/>
+    <row r="651"/>
+    <row r="652"/>
+    <row r="653"/>
+    <row r="654"/>
+    <row r="655"/>
+    <row r="656"/>
+    <row r="657"/>
+    <row r="658"/>
+    <row r="659"/>
+    <row r="660"/>
+    <row r="661"/>
+    <row r="662"/>
+    <row r="663"/>
+    <row r="664"/>
+    <row r="665"/>
+    <row r="666"/>
+    <row r="667"/>
+    <row r="668"/>
+    <row r="669"/>
+    <row r="670"/>
+    <row r="671"/>
+    <row r="672"/>
+    <row r="673"/>
+    <row r="674"/>
+    <row r="675"/>
+    <row r="676"/>
+    <row r="677"/>
+    <row r="678"/>
+    <row r="679"/>
+    <row r="680"/>
+    <row r="681"/>
+    <row r="682"/>
+    <row r="683"/>
+    <row r="684"/>
+    <row r="685"/>
+    <row r="686"/>
+    <row r="687"/>
+    <row r="688"/>
+    <row r="689"/>
+    <row r="690"/>
+    <row r="691"/>
+    <row r="692"/>
+    <row r="693"/>
+    <row r="694"/>
+    <row r="695"/>
+    <row r="696"/>
+    <row r="697"/>
+    <row r="698"/>
+    <row r="699"/>
+    <row r="700"/>
+    <row r="701"/>
+    <row r="702"/>
+    <row r="703"/>
+    <row r="704"/>
+    <row r="705"/>
+    <row r="706"/>
+    <row r="707"/>
+    <row r="708"/>
+    <row r="709"/>
+    <row r="710"/>
+    <row r="711"/>
+    <row r="712"/>
+    <row r="713"/>
+    <row r="714"/>
+    <row r="715"/>
+    <row r="716"/>
+    <row r="717"/>
+    <row r="718"/>
+    <row r="719"/>
+    <row r="720"/>
+    <row r="721"/>
+    <row r="722"/>
+    <row r="723"/>
+    <row r="724"/>
+    <row r="725"/>
+    <row r="726"/>
+    <row r="727"/>
+    <row r="728"/>
+    <row r="729"/>
+    <row r="730"/>
+    <row r="731"/>
+    <row r="732"/>
+    <row r="733"/>
+    <row r="734"/>
+    <row r="735"/>
+    <row r="736"/>
+    <row r="737"/>
+    <row r="738"/>
+    <row r="739"/>
+    <row r="740"/>
+    <row r="741"/>
+    <row r="742"/>
+    <row r="743"/>
+    <row r="744"/>
+    <row r="745"/>
+    <row r="746"/>
+    <row r="747"/>
+    <row r="748"/>
+    <row r="749"/>
+    <row r="750"/>
+    <row r="751"/>
+    <row r="752"/>
+    <row r="753"/>
+    <row r="754"/>
+    <row r="755"/>
+    <row r="756"/>
+    <row r="757"/>
+    <row r="758"/>
+    <row r="759"/>
+    <row r="760"/>
+    <row r="761"/>
+    <row r="762"/>
+    <row r="763"/>
+    <row r="764"/>
+    <row r="765"/>
+    <row r="766"/>
+    <row r="767"/>
+    <row r="768"/>
+    <row r="769"/>
+    <row r="770"/>
+    <row r="771"/>
+    <row r="772"/>
+    <row r="773"/>
+    <row r="774"/>
+    <row r="775"/>
+    <row r="776"/>
+    <row r="777"/>
+    <row r="778"/>
+    <row r="779"/>
+    <row r="780"/>
+    <row r="781"/>
+    <row r="782"/>
+    <row r="783"/>
+    <row r="784"/>
+    <row r="785"/>
+    <row r="786"/>
+    <row r="787"/>
+    <row r="788"/>
+    <row r="789"/>
+    <row r="790"/>
+    <row r="791"/>
+    <row r="792"/>
+    <row r="793"/>
+    <row r="794"/>
+    <row r="795"/>
+    <row r="796"/>
+    <row r="797"/>
+    <row r="798"/>
+    <row r="799"/>
+    <row r="800"/>
+    <row r="801"/>
+    <row r="802"/>
+    <row r="803"/>
+    <row r="804"/>
+    <row r="805"/>
+    <row r="806"/>
+    <row r="807"/>
+    <row r="808"/>
+    <row r="809"/>
+    <row r="810"/>
+    <row r="811"/>
+    <row r="812"/>
+    <row r="813"/>
+    <row r="814"/>
+    <row r="815"/>
+    <row r="816"/>
+    <row r="817"/>
+    <row r="818"/>
+    <row r="819"/>
+    <row r="820"/>
+    <row r="821"/>
+    <row r="822"/>
+    <row r="823"/>
+    <row r="824"/>
+    <row r="825"/>
+    <row r="826"/>
+    <row r="827"/>
+    <row r="828"/>
+    <row r="829"/>
+    <row r="830"/>
+    <row r="831"/>
+    <row r="832"/>
+    <row r="833"/>
+    <row r="834"/>
+    <row r="835"/>
+    <row r="836"/>
+    <row r="837"/>
+    <row r="838"/>
+    <row r="839"/>
+    <row r="840"/>
+    <row r="841"/>
+    <row r="842"/>
+    <row r="843"/>
+    <row r="844"/>
+    <row r="845"/>
+    <row r="846"/>
+    <row r="847"/>
+    <row r="848"/>
+    <row r="849"/>
+    <row r="850"/>
+    <row r="851"/>
+    <row r="852"/>
+    <row r="853"/>
+    <row r="854"/>
+    <row r="855"/>
+    <row r="856"/>
+    <row r="857"/>
+    <row r="858"/>
+    <row r="859"/>
+    <row r="860"/>
+    <row r="861"/>
+    <row r="862"/>
+    <row r="863"/>
+    <row r="864"/>
+    <row r="865"/>
+    <row r="866"/>
+    <row r="867"/>
+    <row r="868"/>
+    <row r="869"/>
+    <row r="870"/>
+    <row r="871"/>
+    <row r="872"/>
+    <row r="873"/>
+    <row r="874"/>
+    <row r="875"/>
+    <row r="876"/>
+    <row r="877"/>
+    <row r="878"/>
+    <row r="879"/>
+    <row r="880"/>
+    <row r="881"/>
+    <row r="882"/>
+    <row r="883"/>
+    <row r="884"/>
+    <row r="885"/>
+    <row r="886"/>
+    <row r="887"/>
+    <row r="888"/>
+    <row r="889"/>
+    <row r="890"/>
+    <row r="891"/>
+    <row r="892"/>
+    <row r="893"/>
+    <row r="894"/>
+    <row r="895"/>
+    <row r="896"/>
+    <row r="897"/>
+    <row r="898"/>
+    <row r="899"/>
+    <row r="900"/>
+    <row r="901"/>
+    <row r="902"/>
+    <row r="903"/>
+    <row r="904"/>
+    <row r="905"/>
+    <row r="906"/>
+    <row r="907"/>
+    <row r="908"/>
+    <row r="909"/>
+    <row r="910"/>
+    <row r="911"/>
+    <row r="912"/>
+    <row r="913"/>
+    <row r="914"/>
+    <row r="915"/>
+    <row r="916"/>
+    <row r="917"/>
+    <row r="918"/>
+    <row r="919"/>
+    <row r="920"/>
+    <row r="921"/>
+    <row r="922"/>
+    <row r="923"/>
+    <row r="924"/>
+    <row r="925"/>
+    <row r="926"/>
+    <row r="927"/>
+    <row r="928"/>
+    <row r="929"/>
+    <row r="930"/>
+    <row r="931"/>
+    <row r="932"/>
+    <row r="933"/>
+    <row r="934"/>
+    <row r="935"/>
+    <row r="936"/>
+    <row r="937"/>
+    <row r="938"/>
+    <row r="939"/>
+    <row r="940"/>
+    <row r="941"/>
+    <row r="942"/>
+    <row r="943"/>
+    <row r="944"/>
+    <row r="945"/>
+    <row r="946"/>
+    <row r="947"/>
+    <row r="948"/>
+    <row r="949"/>
+    <row r="950"/>
+    <row r="951"/>
+    <row r="952"/>
+    <row r="953"/>
+    <row r="954"/>
+    <row r="955"/>
+    <row r="956"/>
+    <row r="957"/>
+    <row r="958"/>
+    <row r="959"/>
+    <row r="960"/>
+    <row r="961"/>
+    <row r="962"/>
+    <row r="963"/>
+    <row r="964"/>
+    <row r="965"/>
+    <row r="966"/>
+    <row r="967"/>
+    <row r="968"/>
+    <row r="969"/>
+    <row r="970"/>
+    <row r="971"/>
+    <row r="972"/>
+    <row r="973"/>
+    <row r="974"/>
+    <row r="975"/>
+    <row r="976"/>
+    <row r="977"/>
+    <row r="978"/>
+    <row r="979"/>
+    <row r="980"/>
+    <row r="981"/>
+    <row r="982"/>
+    <row r="983"/>
+    <row r="984"/>
+    <row r="985"/>
+    <row r="986"/>
+    <row r="987"/>
+    <row r="988"/>
+    <row r="989"/>
+    <row r="990"/>
+    <row r="991"/>
+    <row r="992"/>
+    <row r="993"/>
+    <row r="994"/>
+    <row r="995"/>
+    <row r="996"/>
+    <row r="997"/>
+    <row r="998"/>
+    <row r="999"/>
+    <row r="1000"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -556,7 +1456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A100"/>
+  <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -688,6 +1588,906 @@
     <row r="98"/>
     <row r="99"/>
     <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
+    <row r="170"/>
+    <row r="171"/>
+    <row r="172"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189"/>
+    <row r="190"/>
+    <row r="191"/>
+    <row r="192"/>
+    <row r="193"/>
+    <row r="194"/>
+    <row r="195"/>
+    <row r="196"/>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200"/>
+    <row r="201"/>
+    <row r="202"/>
+    <row r="203"/>
+    <row r="204"/>
+    <row r="205"/>
+    <row r="206"/>
+    <row r="207"/>
+    <row r="208"/>
+    <row r="209"/>
+    <row r="210"/>
+    <row r="211"/>
+    <row r="212"/>
+    <row r="213"/>
+    <row r="214"/>
+    <row r="215"/>
+    <row r="216"/>
+    <row r="217"/>
+    <row r="218"/>
+    <row r="219"/>
+    <row r="220"/>
+    <row r="221"/>
+    <row r="222"/>
+    <row r="223"/>
+    <row r="224"/>
+    <row r="225"/>
+    <row r="226"/>
+    <row r="227"/>
+    <row r="228"/>
+    <row r="229"/>
+    <row r="230"/>
+    <row r="231"/>
+    <row r="232"/>
+    <row r="233"/>
+    <row r="234"/>
+    <row r="235"/>
+    <row r="236"/>
+    <row r="237"/>
+    <row r="238"/>
+    <row r="239"/>
+    <row r="240"/>
+    <row r="241"/>
+    <row r="242"/>
+    <row r="243"/>
+    <row r="244"/>
+    <row r="245"/>
+    <row r="246"/>
+    <row r="247"/>
+    <row r="248"/>
+    <row r="249"/>
+    <row r="250"/>
+    <row r="251"/>
+    <row r="252"/>
+    <row r="253"/>
+    <row r="254"/>
+    <row r="255"/>
+    <row r="256"/>
+    <row r="257"/>
+    <row r="258"/>
+    <row r="259"/>
+    <row r="260"/>
+    <row r="261"/>
+    <row r="262"/>
+    <row r="263"/>
+    <row r="264"/>
+    <row r="265"/>
+    <row r="266"/>
+    <row r="267"/>
+    <row r="268"/>
+    <row r="269"/>
+    <row r="270"/>
+    <row r="271"/>
+    <row r="272"/>
+    <row r="273"/>
+    <row r="274"/>
+    <row r="275"/>
+    <row r="276"/>
+    <row r="277"/>
+    <row r="278"/>
+    <row r="279"/>
+    <row r="280"/>
+    <row r="281"/>
+    <row r="282"/>
+    <row r="283"/>
+    <row r="284"/>
+    <row r="285"/>
+    <row r="286"/>
+    <row r="287"/>
+    <row r="288"/>
+    <row r="289"/>
+    <row r="290"/>
+    <row r="291"/>
+    <row r="292"/>
+    <row r="293"/>
+    <row r="294"/>
+    <row r="295"/>
+    <row r="296"/>
+    <row r="297"/>
+    <row r="298"/>
+    <row r="299"/>
+    <row r="300"/>
+    <row r="301"/>
+    <row r="302"/>
+    <row r="303"/>
+    <row r="304"/>
+    <row r="305"/>
+    <row r="306"/>
+    <row r="307"/>
+    <row r="308"/>
+    <row r="309"/>
+    <row r="310"/>
+    <row r="311"/>
+    <row r="312"/>
+    <row r="313"/>
+    <row r="314"/>
+    <row r="315"/>
+    <row r="316"/>
+    <row r="317"/>
+    <row r="318"/>
+    <row r="319"/>
+    <row r="320"/>
+    <row r="321"/>
+    <row r="322"/>
+    <row r="323"/>
+    <row r="324"/>
+    <row r="325"/>
+    <row r="326"/>
+    <row r="327"/>
+    <row r="328"/>
+    <row r="329"/>
+    <row r="330"/>
+    <row r="331"/>
+    <row r="332"/>
+    <row r="333"/>
+    <row r="334"/>
+    <row r="335"/>
+    <row r="336"/>
+    <row r="337"/>
+    <row r="338"/>
+    <row r="339"/>
+    <row r="340"/>
+    <row r="341"/>
+    <row r="342"/>
+    <row r="343"/>
+    <row r="344"/>
+    <row r="345"/>
+    <row r="346"/>
+    <row r="347"/>
+    <row r="348"/>
+    <row r="349"/>
+    <row r="350"/>
+    <row r="351"/>
+    <row r="352"/>
+    <row r="353"/>
+    <row r="354"/>
+    <row r="355"/>
+    <row r="356"/>
+    <row r="357"/>
+    <row r="358"/>
+    <row r="359"/>
+    <row r="360"/>
+    <row r="361"/>
+    <row r="362"/>
+    <row r="363"/>
+    <row r="364"/>
+    <row r="365"/>
+    <row r="366"/>
+    <row r="367"/>
+    <row r="368"/>
+    <row r="369"/>
+    <row r="370"/>
+    <row r="371"/>
+    <row r="372"/>
+    <row r="373"/>
+    <row r="374"/>
+    <row r="375"/>
+    <row r="376"/>
+    <row r="377"/>
+    <row r="378"/>
+    <row r="379"/>
+    <row r="380"/>
+    <row r="381"/>
+    <row r="382"/>
+    <row r="383"/>
+    <row r="384"/>
+    <row r="385"/>
+    <row r="386"/>
+    <row r="387"/>
+    <row r="388"/>
+    <row r="389"/>
+    <row r="390"/>
+    <row r="391"/>
+    <row r="392"/>
+    <row r="393"/>
+    <row r="394"/>
+    <row r="395"/>
+    <row r="396"/>
+    <row r="397"/>
+    <row r="398"/>
+    <row r="399"/>
+    <row r="400"/>
+    <row r="401"/>
+    <row r="402"/>
+    <row r="403"/>
+    <row r="404"/>
+    <row r="405"/>
+    <row r="406"/>
+    <row r="407"/>
+    <row r="408"/>
+    <row r="409"/>
+    <row r="410"/>
+    <row r="411"/>
+    <row r="412"/>
+    <row r="413"/>
+    <row r="414"/>
+    <row r="415"/>
+    <row r="416"/>
+    <row r="417"/>
+    <row r="418"/>
+    <row r="419"/>
+    <row r="420"/>
+    <row r="421"/>
+    <row r="422"/>
+    <row r="423"/>
+    <row r="424"/>
+    <row r="425"/>
+    <row r="426"/>
+    <row r="427"/>
+    <row r="428"/>
+    <row r="429"/>
+    <row r="430"/>
+    <row r="431"/>
+    <row r="432"/>
+    <row r="433"/>
+    <row r="434"/>
+    <row r="435"/>
+    <row r="436"/>
+    <row r="437"/>
+    <row r="438"/>
+    <row r="439"/>
+    <row r="440"/>
+    <row r="441"/>
+    <row r="442"/>
+    <row r="443"/>
+    <row r="444"/>
+    <row r="445"/>
+    <row r="446"/>
+    <row r="447"/>
+    <row r="448"/>
+    <row r="449"/>
+    <row r="450"/>
+    <row r="451"/>
+    <row r="452"/>
+    <row r="453"/>
+    <row r="454"/>
+    <row r="455"/>
+    <row r="456"/>
+    <row r="457"/>
+    <row r="458"/>
+    <row r="459"/>
+    <row r="460"/>
+    <row r="461"/>
+    <row r="462"/>
+    <row r="463"/>
+    <row r="464"/>
+    <row r="465"/>
+    <row r="466"/>
+    <row r="467"/>
+    <row r="468"/>
+    <row r="469"/>
+    <row r="470"/>
+    <row r="471"/>
+    <row r="472"/>
+    <row r="473"/>
+    <row r="474"/>
+    <row r="475"/>
+    <row r="476"/>
+    <row r="477"/>
+    <row r="478"/>
+    <row r="479"/>
+    <row r="480"/>
+    <row r="481"/>
+    <row r="482"/>
+    <row r="483"/>
+    <row r="484"/>
+    <row r="485"/>
+    <row r="486"/>
+    <row r="487"/>
+    <row r="488"/>
+    <row r="489"/>
+    <row r="490"/>
+    <row r="491"/>
+    <row r="492"/>
+    <row r="493"/>
+    <row r="494"/>
+    <row r="495"/>
+    <row r="496"/>
+    <row r="497"/>
+    <row r="498"/>
+    <row r="499"/>
+    <row r="500"/>
+    <row r="501"/>
+    <row r="502"/>
+    <row r="503"/>
+    <row r="504"/>
+    <row r="505"/>
+    <row r="506"/>
+    <row r="507"/>
+    <row r="508"/>
+    <row r="509"/>
+    <row r="510"/>
+    <row r="511"/>
+    <row r="512"/>
+    <row r="513"/>
+    <row r="514"/>
+    <row r="515"/>
+    <row r="516"/>
+    <row r="517"/>
+    <row r="518"/>
+    <row r="519"/>
+    <row r="520"/>
+    <row r="521"/>
+    <row r="522"/>
+    <row r="523"/>
+    <row r="524"/>
+    <row r="525"/>
+    <row r="526"/>
+    <row r="527"/>
+    <row r="528"/>
+    <row r="529"/>
+    <row r="530"/>
+    <row r="531"/>
+    <row r="532"/>
+    <row r="533"/>
+    <row r="534"/>
+    <row r="535"/>
+    <row r="536"/>
+    <row r="537"/>
+    <row r="538"/>
+    <row r="539"/>
+    <row r="540"/>
+    <row r="541"/>
+    <row r="542"/>
+    <row r="543"/>
+    <row r="544"/>
+    <row r="545"/>
+    <row r="546"/>
+    <row r="547"/>
+    <row r="548"/>
+    <row r="549"/>
+    <row r="550"/>
+    <row r="551"/>
+    <row r="552"/>
+    <row r="553"/>
+    <row r="554"/>
+    <row r="555"/>
+    <row r="556"/>
+    <row r="557"/>
+    <row r="558"/>
+    <row r="559"/>
+    <row r="560"/>
+    <row r="561"/>
+    <row r="562"/>
+    <row r="563"/>
+    <row r="564"/>
+    <row r="565"/>
+    <row r="566"/>
+    <row r="567"/>
+    <row r="568"/>
+    <row r="569"/>
+    <row r="570"/>
+    <row r="571"/>
+    <row r="572"/>
+    <row r="573"/>
+    <row r="574"/>
+    <row r="575"/>
+    <row r="576"/>
+    <row r="577"/>
+    <row r="578"/>
+    <row r="579"/>
+    <row r="580"/>
+    <row r="581"/>
+    <row r="582"/>
+    <row r="583"/>
+    <row r="584"/>
+    <row r="585"/>
+    <row r="586"/>
+    <row r="587"/>
+    <row r="588"/>
+    <row r="589"/>
+    <row r="590"/>
+    <row r="591"/>
+    <row r="592"/>
+    <row r="593"/>
+    <row r="594"/>
+    <row r="595"/>
+    <row r="596"/>
+    <row r="597"/>
+    <row r="598"/>
+    <row r="599"/>
+    <row r="600"/>
+    <row r="601"/>
+    <row r="602"/>
+    <row r="603"/>
+    <row r="604"/>
+    <row r="605"/>
+    <row r="606"/>
+    <row r="607"/>
+    <row r="608"/>
+    <row r="609"/>
+    <row r="610"/>
+    <row r="611"/>
+    <row r="612"/>
+    <row r="613"/>
+    <row r="614"/>
+    <row r="615"/>
+    <row r="616"/>
+    <row r="617"/>
+    <row r="618"/>
+    <row r="619"/>
+    <row r="620"/>
+    <row r="621"/>
+    <row r="622"/>
+    <row r="623"/>
+    <row r="624"/>
+    <row r="625"/>
+    <row r="626"/>
+    <row r="627"/>
+    <row r="628"/>
+    <row r="629"/>
+    <row r="630"/>
+    <row r="631"/>
+    <row r="632"/>
+    <row r="633"/>
+    <row r="634"/>
+    <row r="635"/>
+    <row r="636"/>
+    <row r="637"/>
+    <row r="638"/>
+    <row r="639"/>
+    <row r="640"/>
+    <row r="641"/>
+    <row r="642"/>
+    <row r="643"/>
+    <row r="644"/>
+    <row r="645"/>
+    <row r="646"/>
+    <row r="647"/>
+    <row r="648"/>
+    <row r="649"/>
+    <row r="650"/>
+    <row r="651"/>
+    <row r="652"/>
+    <row r="653"/>
+    <row r="654"/>
+    <row r="655"/>
+    <row r="656"/>
+    <row r="657"/>
+    <row r="658"/>
+    <row r="659"/>
+    <row r="660"/>
+    <row r="661"/>
+    <row r="662"/>
+    <row r="663"/>
+    <row r="664"/>
+    <row r="665"/>
+    <row r="666"/>
+    <row r="667"/>
+    <row r="668"/>
+    <row r="669"/>
+    <row r="670"/>
+    <row r="671"/>
+    <row r="672"/>
+    <row r="673"/>
+    <row r="674"/>
+    <row r="675"/>
+    <row r="676"/>
+    <row r="677"/>
+    <row r="678"/>
+    <row r="679"/>
+    <row r="680"/>
+    <row r="681"/>
+    <row r="682"/>
+    <row r="683"/>
+    <row r="684"/>
+    <row r="685"/>
+    <row r="686"/>
+    <row r="687"/>
+    <row r="688"/>
+    <row r="689"/>
+    <row r="690"/>
+    <row r="691"/>
+    <row r="692"/>
+    <row r="693"/>
+    <row r="694"/>
+    <row r="695"/>
+    <row r="696"/>
+    <row r="697"/>
+    <row r="698"/>
+    <row r="699"/>
+    <row r="700"/>
+    <row r="701"/>
+    <row r="702"/>
+    <row r="703"/>
+    <row r="704"/>
+    <row r="705"/>
+    <row r="706"/>
+    <row r="707"/>
+    <row r="708"/>
+    <row r="709"/>
+    <row r="710"/>
+    <row r="711"/>
+    <row r="712"/>
+    <row r="713"/>
+    <row r="714"/>
+    <row r="715"/>
+    <row r="716"/>
+    <row r="717"/>
+    <row r="718"/>
+    <row r="719"/>
+    <row r="720"/>
+    <row r="721"/>
+    <row r="722"/>
+    <row r="723"/>
+    <row r="724"/>
+    <row r="725"/>
+    <row r="726"/>
+    <row r="727"/>
+    <row r="728"/>
+    <row r="729"/>
+    <row r="730"/>
+    <row r="731"/>
+    <row r="732"/>
+    <row r="733"/>
+    <row r="734"/>
+    <row r="735"/>
+    <row r="736"/>
+    <row r="737"/>
+    <row r="738"/>
+    <row r="739"/>
+    <row r="740"/>
+    <row r="741"/>
+    <row r="742"/>
+    <row r="743"/>
+    <row r="744"/>
+    <row r="745"/>
+    <row r="746"/>
+    <row r="747"/>
+    <row r="748"/>
+    <row r="749"/>
+    <row r="750"/>
+    <row r="751"/>
+    <row r="752"/>
+    <row r="753"/>
+    <row r="754"/>
+    <row r="755"/>
+    <row r="756"/>
+    <row r="757"/>
+    <row r="758"/>
+    <row r="759"/>
+    <row r="760"/>
+    <row r="761"/>
+    <row r="762"/>
+    <row r="763"/>
+    <row r="764"/>
+    <row r="765"/>
+    <row r="766"/>
+    <row r="767"/>
+    <row r="768"/>
+    <row r="769"/>
+    <row r="770"/>
+    <row r="771"/>
+    <row r="772"/>
+    <row r="773"/>
+    <row r="774"/>
+    <row r="775"/>
+    <row r="776"/>
+    <row r="777"/>
+    <row r="778"/>
+    <row r="779"/>
+    <row r="780"/>
+    <row r="781"/>
+    <row r="782"/>
+    <row r="783"/>
+    <row r="784"/>
+    <row r="785"/>
+    <row r="786"/>
+    <row r="787"/>
+    <row r="788"/>
+    <row r="789"/>
+    <row r="790"/>
+    <row r="791"/>
+    <row r="792"/>
+    <row r="793"/>
+    <row r="794"/>
+    <row r="795"/>
+    <row r="796"/>
+    <row r="797"/>
+    <row r="798"/>
+    <row r="799"/>
+    <row r="800"/>
+    <row r="801"/>
+    <row r="802"/>
+    <row r="803"/>
+    <row r="804"/>
+    <row r="805"/>
+    <row r="806"/>
+    <row r="807"/>
+    <row r="808"/>
+    <row r="809"/>
+    <row r="810"/>
+    <row r="811"/>
+    <row r="812"/>
+    <row r="813"/>
+    <row r="814"/>
+    <row r="815"/>
+    <row r="816"/>
+    <row r="817"/>
+    <row r="818"/>
+    <row r="819"/>
+    <row r="820"/>
+    <row r="821"/>
+    <row r="822"/>
+    <row r="823"/>
+    <row r="824"/>
+    <row r="825"/>
+    <row r="826"/>
+    <row r="827"/>
+    <row r="828"/>
+    <row r="829"/>
+    <row r="830"/>
+    <row r="831"/>
+    <row r="832"/>
+    <row r="833"/>
+    <row r="834"/>
+    <row r="835"/>
+    <row r="836"/>
+    <row r="837"/>
+    <row r="838"/>
+    <row r="839"/>
+    <row r="840"/>
+    <row r="841"/>
+    <row r="842"/>
+    <row r="843"/>
+    <row r="844"/>
+    <row r="845"/>
+    <row r="846"/>
+    <row r="847"/>
+    <row r="848"/>
+    <row r="849"/>
+    <row r="850"/>
+    <row r="851"/>
+    <row r="852"/>
+    <row r="853"/>
+    <row r="854"/>
+    <row r="855"/>
+    <row r="856"/>
+    <row r="857"/>
+    <row r="858"/>
+    <row r="859"/>
+    <row r="860"/>
+    <row r="861"/>
+    <row r="862"/>
+    <row r="863"/>
+    <row r="864"/>
+    <row r="865"/>
+    <row r="866"/>
+    <row r="867"/>
+    <row r="868"/>
+    <row r="869"/>
+    <row r="870"/>
+    <row r="871"/>
+    <row r="872"/>
+    <row r="873"/>
+    <row r="874"/>
+    <row r="875"/>
+    <row r="876"/>
+    <row r="877"/>
+    <row r="878"/>
+    <row r="879"/>
+    <row r="880"/>
+    <row r="881"/>
+    <row r="882"/>
+    <row r="883"/>
+    <row r="884"/>
+    <row r="885"/>
+    <row r="886"/>
+    <row r="887"/>
+    <row r="888"/>
+    <row r="889"/>
+    <row r="890"/>
+    <row r="891"/>
+    <row r="892"/>
+    <row r="893"/>
+    <row r="894"/>
+    <row r="895"/>
+    <row r="896"/>
+    <row r="897"/>
+    <row r="898"/>
+    <row r="899"/>
+    <row r="900"/>
+    <row r="901"/>
+    <row r="902"/>
+    <row r="903"/>
+    <row r="904"/>
+    <row r="905"/>
+    <row r="906"/>
+    <row r="907"/>
+    <row r="908"/>
+    <row r="909"/>
+    <row r="910"/>
+    <row r="911"/>
+    <row r="912"/>
+    <row r="913"/>
+    <row r="914"/>
+    <row r="915"/>
+    <row r="916"/>
+    <row r="917"/>
+    <row r="918"/>
+    <row r="919"/>
+    <row r="920"/>
+    <row r="921"/>
+    <row r="922"/>
+    <row r="923"/>
+    <row r="924"/>
+    <row r="925"/>
+    <row r="926"/>
+    <row r="927"/>
+    <row r="928"/>
+    <row r="929"/>
+    <row r="930"/>
+    <row r="931"/>
+    <row r="932"/>
+    <row r="933"/>
+    <row r="934"/>
+    <row r="935"/>
+    <row r="936"/>
+    <row r="937"/>
+    <row r="938"/>
+    <row r="939"/>
+    <row r="940"/>
+    <row r="941"/>
+    <row r="942"/>
+    <row r="943"/>
+    <row r="944"/>
+    <row r="945"/>
+    <row r="946"/>
+    <row r="947"/>
+    <row r="948"/>
+    <row r="949"/>
+    <row r="950"/>
+    <row r="951"/>
+    <row r="952"/>
+    <row r="953"/>
+    <row r="954"/>
+    <row r="955"/>
+    <row r="956"/>
+    <row r="957"/>
+    <row r="958"/>
+    <row r="959"/>
+    <row r="960"/>
+    <row r="961"/>
+    <row r="962"/>
+    <row r="963"/>
+    <row r="964"/>
+    <row r="965"/>
+    <row r="966"/>
+    <row r="967"/>
+    <row r="968"/>
+    <row r="969"/>
+    <row r="970"/>
+    <row r="971"/>
+    <row r="972"/>
+    <row r="973"/>
+    <row r="974"/>
+    <row r="975"/>
+    <row r="976"/>
+    <row r="977"/>
+    <row r="978"/>
+    <row r="979"/>
+    <row r="980"/>
+    <row r="981"/>
+    <row r="982"/>
+    <row r="983"/>
+    <row r="984"/>
+    <row r="985"/>
+    <row r="986"/>
+    <row r="987"/>
+    <row r="988"/>
+    <row r="989"/>
+    <row r="990"/>
+    <row r="991"/>
+    <row r="992"/>
+    <row r="993"/>
+    <row r="994"/>
+    <row r="995"/>
+    <row r="996"/>
+    <row r="997"/>
+    <row r="998"/>
+    <row r="999"/>
+    <row r="1000"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Python only writes fields to excel file if checked
</commit_message>
<xml_diff>
--- a/docs/output/OutputDataDefinition.xlsx
+++ b/docs/output/OutputDataDefinition.xlsx
@@ -440,13 +440,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-    </row>
+    <row r="2"/>
     <row r="3"/>
     <row r="4"/>
     <row r="5"/>
@@ -1467,31 +1461,13 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>T1F1</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
           <t>T1F2</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>T2F1</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>T2F2</t>
-        </is>
-      </c>
-    </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
     <row r="5"/>
     <row r="6"/>
     <row r="7"/>

</xml_diff>

<commit_message>
Groudwork for file upload and parsing
</commit_message>
<xml_diff>
--- a/docs/output/OutputDataDefinition.xlsx
+++ b/docs/output/OutputDataDefinition.xlsx
@@ -433,13 +433,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-    </row>
+    <row r="1"/>
     <row r="2"/>
     <row r="3"/>
     <row r="4"/>
@@ -1458,13 +1452,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>T1F2</t>
-        </is>
-      </c>
-    </row>
+    <row r="1"/>
     <row r="2"/>
     <row r="3"/>
     <row r="4"/>

</xml_diff>

<commit_message>
Checkboxes now updating after state changes.
</commit_message>
<xml_diff>
--- a/docs/output/OutputDataDefinition.xlsx
+++ b/docs/output/OutputDataDefinition.xlsx
@@ -433,9 +433,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1"/>
-    <row r="2"/>
-    <row r="3"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>TestTable1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TestTable2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TestTable3</t>
+        </is>
+      </c>
+    </row>
     <row r="4"/>
     <row r="5"/>
     <row r="6"/>
@@ -1452,15 +1470,69 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1"/>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>TestValue1.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TestValue1.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TestValue1.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TestValue2.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TestValue2.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TestValue3.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TestValue3.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TestValue3.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>TestValue3.4</t>
+        </is>
+      </c>
+    </row>
     <row r="10"/>
     <row r="11"/>
     <row r="12"/>

</xml_diff>

<commit_message>
Update to UX layout
</commit_message>
<xml_diff>
--- a/docs/output/OutputDataDefinition.xlsx
+++ b/docs/output/OutputDataDefinition.xlsx
@@ -450,7 +450,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TestTable3</t>
+          <t>T4</t>
         </is>
       </c>
     </row>
@@ -1505,34 +1505,10 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>TestValue3.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>TestValue3.2</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>TestValue3.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>TestValue3.4</t>
-        </is>
-      </c>
-    </row>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
     <row r="10"/>
     <row r="11"/>
     <row r="12"/>

</xml_diff>

<commit_message>
Read with and without checkboxes
</commit_message>
<xml_diff>
--- a/docs/output/OutputDataDefinition.xlsx
+++ b/docs/output/OutputDataDefinition.xlsx
@@ -436,24 +436,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TestTable1</t>
+          <t>T2</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>TestTable2</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>T4</t>
-        </is>
-      </c>
-    </row>
+    <row r="2"/>
+    <row r="3"/>
     <row r="4"/>
     <row r="5"/>
     <row r="6"/>
@@ -1470,41 +1458,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>TestValue1.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>TestValue1.2</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>TestValue1.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>TestValue2.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>TestValue2.2</t>
-        </is>
-      </c>
-    </row>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
     <row r="6"/>
     <row r="7"/>
     <row r="8"/>

</xml_diff>

<commit_message>
Make update to field save state.
</commit_message>
<xml_diff>
--- a/docs/output/OutputDataDefinition.xlsx
+++ b/docs/output/OutputDataDefinition.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>T1</t>
         </is>
       </c>
     </row>
@@ -1458,7 +1458,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>T1F2</t>
+        </is>
+      </c>
+    </row>
     <row r="2"/>
     <row r="3"/>
     <row r="4"/>

</xml_diff>